<commit_message>
Update bracing coord. tables based on selection
</commit_message>
<xml_diff>
--- a/Test Files/autobuilder - v2/newReadFile.xlsx
+++ b/Test Files/autobuilder - v2/newReadFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/shuocheng_zhang_mail_utoronto_ca/Documents/Desktop/Seismic/Autobuilder-3.0/Test Files/autobuilder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/shuocheng_zhang_mail_utoronto_ca/Documents/Desktop/Seismic/Autobuilder-3.0/Test Files/autobuilder - v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{927F850D-60C7-403D-92D7-D99B5A94C16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{239F7BD1-C896-4C52-9A9A-2D8FBDC08AE5}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{927F850D-60C7-403D-92D7-D99B5A94C16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{02C3D969-BA1B-4327-8E4A-EF2CC73ADE89}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="577" activeTab="3" xr2:uid="{94F6AF0B-8232-48E5-84EE-C3EAE4AA8963}"/>
+    <workbookView xWindow="0" yWindow="570" windowWidth="14400" windowHeight="15030" tabRatio="577" firstSheet="2" activeTab="3" xr2:uid="{94F6AF0B-8232-48E5-84EE-C3EAE4AA8963}"/>
   </bookViews>
   <sheets>
     <sheet name="bracing" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="55">
   <si>
     <t>material</t>
   </si>
@@ -203,198 +203,6 @@
   </si>
   <si>
     <t>V1</t>
-  </si>
-  <si>
-    <t>V2</t>
-  </si>
-  <si>
-    <t>V3</t>
-  </si>
-  <si>
-    <t>V4</t>
-  </si>
-  <si>
-    <t>V5</t>
-  </si>
-  <si>
-    <t>V6</t>
-  </si>
-  <si>
-    <t>V7</t>
-  </si>
-  <si>
-    <t>V8</t>
-  </si>
-  <si>
-    <t>V9</t>
-  </si>
-  <si>
-    <t>V10</t>
-  </si>
-  <si>
-    <t>V11</t>
-  </si>
-  <si>
-    <t>V12</t>
-  </si>
-  <si>
-    <t>V13</t>
-  </si>
-  <si>
-    <t>V14</t>
-  </si>
-  <si>
-    <t>V15</t>
-  </si>
-  <si>
-    <t>V16</t>
-  </si>
-  <si>
-    <t>V17</t>
-  </si>
-  <si>
-    <t>V18</t>
-  </si>
-  <si>
-    <t>V19</t>
-  </si>
-  <si>
-    <t>V20</t>
-  </si>
-  <si>
-    <t>V21</t>
-  </si>
-  <si>
-    <t>V22</t>
-  </si>
-  <si>
-    <t>V23</t>
-  </si>
-  <si>
-    <t>V24</t>
-  </si>
-  <si>
-    <t>V25</t>
-  </si>
-  <si>
-    <t>V26</t>
-  </si>
-  <si>
-    <t>V27</t>
-  </si>
-  <si>
-    <t>V28</t>
-  </si>
-  <si>
-    <t>V29</t>
-  </si>
-  <si>
-    <t>V30</t>
-  </si>
-  <si>
-    <t>V31</t>
-  </si>
-  <si>
-    <t>V32</t>
-  </si>
-  <si>
-    <t>V33</t>
-  </si>
-  <si>
-    <t>V34</t>
-  </si>
-  <si>
-    <t>V35</t>
-  </si>
-  <si>
-    <t>V36</t>
-  </si>
-  <si>
-    <t>V37</t>
-  </si>
-  <si>
-    <t>V38</t>
-  </si>
-  <si>
-    <t>V39</t>
-  </si>
-  <si>
-    <t>V40</t>
-  </si>
-  <si>
-    <t>V41</t>
-  </si>
-  <si>
-    <t>V42</t>
-  </si>
-  <si>
-    <t>V43</t>
-  </si>
-  <si>
-    <t>V44</t>
-  </si>
-  <si>
-    <t>V45</t>
-  </si>
-  <si>
-    <t>V46</t>
-  </si>
-  <si>
-    <t>V47</t>
-  </si>
-  <si>
-    <t>V48</t>
-  </si>
-  <si>
-    <t>V49</t>
-  </si>
-  <si>
-    <t>V50</t>
-  </si>
-  <si>
-    <t>V51</t>
-  </si>
-  <si>
-    <t>V52</t>
-  </si>
-  <si>
-    <t>V53</t>
-  </si>
-  <si>
-    <t>V54</t>
-  </si>
-  <si>
-    <t>V55</t>
-  </si>
-  <si>
-    <t>V56</t>
-  </si>
-  <si>
-    <t>V57</t>
-  </si>
-  <si>
-    <t>V58</t>
-  </si>
-  <si>
-    <t>V59</t>
-  </si>
-  <si>
-    <t>V60</t>
-  </si>
-  <si>
-    <t>V61</t>
-  </si>
-  <si>
-    <t>V62</t>
-  </si>
-  <si>
-    <t>V63</t>
-  </si>
-  <si>
-    <t>V64</t>
-  </si>
-  <si>
-    <t>V65</t>
   </si>
 </sst>
 </file>
@@ -6573,7 +6381,7 @@
   <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6603,7 +6411,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6611,7 +6419,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -6619,7 +6427,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -6627,7 +6435,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -6635,7 +6443,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -6643,7 +6451,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -6651,7 +6459,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -6659,7 +6467,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -6667,7 +6475,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -6675,7 +6483,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -6683,7 +6491,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -6691,7 +6499,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -6699,7 +6507,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -6707,7 +6515,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -6715,7 +6523,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -6723,7 +6531,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -6731,7 +6539,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -6739,7 +6547,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -6747,7 +6555,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -6755,7 +6563,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -6763,7 +6571,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -6771,7 +6579,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -6779,7 +6587,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -6787,7 +6595,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -6795,7 +6603,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -6803,7 +6611,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -6811,7 +6619,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -6819,7 +6627,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -6827,7 +6635,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -6835,7 +6643,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -6843,7 +6651,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -6851,7 +6659,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -6859,7 +6667,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -6867,7 +6675,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -6875,7 +6683,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -6883,7 +6691,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -6891,7 +6699,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -6899,7 +6707,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -6907,7 +6715,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -6915,7 +6723,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -6923,7 +6731,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -6931,7 +6739,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -6939,7 +6747,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -6947,7 +6755,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -6955,7 +6763,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -6963,7 +6771,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -6971,7 +6779,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -6979,7 +6787,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -6987,7 +6795,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -6995,7 +6803,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -7003,7 +6811,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -7011,7 +6819,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -7019,7 +6827,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -7027,7 +6835,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -7035,7 +6843,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -7043,7 +6851,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -7051,7 +6859,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -7059,7 +6867,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>112</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -7067,7 +6875,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -7075,7 +6883,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -7083,7 +6891,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>115</v>
+        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -7091,7 +6899,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -7099,7 +6907,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -7107,7 +6915,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>118</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Bracing Group dialog and debug Assignment dialog
</commit_message>
<xml_diff>
--- a/Test Files/autobuilder - v2/newReadFile.xlsx
+++ b/Test Files/autobuilder - v2/newReadFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/shuocheng_zhang_mail_utoronto_ca/Documents/Desktop/Seismic/Autobuilder-3.0/Test Files/autobuilder - v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{927F850D-60C7-403D-92D7-D99B5A94C16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{02C3D969-BA1B-4327-8E4A-EF2CC73ADE89}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{927F850D-60C7-403D-92D7-D99B5A94C16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{440FD84C-589E-4E92-97F0-D126DF3BC8F6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="570" windowWidth="14400" windowHeight="15030" tabRatio="577" firstSheet="2" activeTab="3" xr2:uid="{94F6AF0B-8232-48E5-84EE-C3EAE4AA8963}"/>
+    <workbookView minimized="1" xWindow="14850" yWindow="825" windowWidth="14025" windowHeight="14055" tabRatio="577" firstSheet="5" activeTab="5" xr2:uid="{94F6AF0B-8232-48E5-84EE-C3EAE4AA8963}"/>
   </bookViews>
   <sheets>
     <sheet name="bracing" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="floorPlan" sheetId="3" r:id="rId3"/>
     <sheet name="bracingAssignment" sheetId="6" r:id="rId4"/>
     <sheet name="projectSettings" sheetId="5" r:id="rId5"/>
+    <sheet name="inputTable" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="59">
   <si>
     <t>material</t>
   </si>
@@ -203,6 +204,18 @@
   </si>
   <si>
     <t>V1</t>
+  </si>
+  <si>
+    <t>Tower</t>
+  </si>
+  <si>
+    <t>Panel</t>
+  </si>
+  <si>
+    <t>Bracing</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
@@ -6380,7 +6393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C44D74-D141-400C-9A83-83919175967E}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
@@ -7018,4 +7031,194 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C99F3A-4389-4710-AC69-74E23E0753CE}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Delete old bracing group dialogs
</commit_message>
<xml_diff>
--- a/Test Files/autobuilder - v2/newReadFile.xlsx
+++ b/Test Files/autobuilder - v2/newReadFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/shuocheng_zhang_mail_utoronto_ca/Documents/Desktop/Seismic/Autobuilder-3.0/Test Files/autobuilder - v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{927F850D-60C7-403D-92D7-D99B5A94C16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{440FD84C-589E-4E92-97F0-D126DF3BC8F6}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="8_{927F850D-60C7-403D-92D7-D99B5A94C16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{22C52593-D9BB-4CEB-9E91-B441001E18CF}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="14850" yWindow="825" windowWidth="14025" windowHeight="14055" tabRatio="577" firstSheet="5" activeTab="5" xr2:uid="{94F6AF0B-8232-48E5-84EE-C3EAE4AA8963}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="577" firstSheet="4" activeTab="5" xr2:uid="{94F6AF0B-8232-48E5-84EE-C3EAE4AA8963}"/>
   </bookViews>
   <sheets>
     <sheet name="bracing" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="bracingAssignment" sheetId="6" r:id="rId4"/>
     <sheet name="projectSettings" sheetId="5" r:id="rId5"/>
     <sheet name="inputTable" sheetId="7" r:id="rId6"/>
+    <sheet name="restrictions" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="55">
   <si>
     <t>material</t>
   </si>
@@ -205,18 +206,6 @@
   <si>
     <t>V1</t>
   </si>
-  <si>
-    <t>Tower</t>
-  </si>
-  <si>
-    <t>Panel</t>
-  </si>
-  <si>
-    <t>Bracing</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
 </sst>
 </file>
 
@@ -275,6 +264,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>53950</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234FE545-2200-4D9F-BEC8-DF84AD246E5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6988150" cy="1924050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7035,190 +7073,32 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C99F3A-4389-4710-AC69-74E23E0753CE}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C17"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-  </sheetData>
+  <cols>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43ABE7CA-99C1-4F9A-A7D3-2F18B37EF36A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Design Variable Dialog
</commit_message>
<xml_diff>
--- a/Test Files/autobuilder - v2/newReadFile.xlsx
+++ b/Test Files/autobuilder - v2/newReadFile.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="85" documentId="8_{927F850D-60C7-403D-92D7-D99B5A94C16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{22C52593-D9BB-4CEB-9E91-B441001E18CF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="577" firstSheet="4" activeTab="5" xr2:uid="{94F6AF0B-8232-48E5-84EE-C3EAE4AA8963}"/>
+    <workbookView minimized="1" xWindow="1470" yWindow="1890" windowWidth="14025" windowHeight="14055" tabRatio="577" firstSheet="4" activeTab="4" xr2:uid="{94F6AF0B-8232-48E5-84EE-C3EAE4AA8963}"/>
   </bookViews>
   <sheets>
     <sheet name="bracing" sheetId="1" r:id="rId1"/>
@@ -6979,8 +6979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12880AED-CC7D-41FF-B7FC-F0390CB22B89}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7075,7 +7075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C99F3A-4389-4710-AC69-74E23E0753CE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>

</xml_diff>